<commit_message>
Test Data Sheet Prefix for UA WebForms
</commit_message>
<xml_diff>
--- a/testData/Execution Status.xlsx
+++ b/testData/Execution Status.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId6"/>
+    <sheet name="User Assignment Scope" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="220">
   <si>
     <t>Condition 1</t>
   </si>
@@ -599,6 +599,117 @@
   </si>
   <si>
     <t>Test Run</t>
+  </si>
+  <si>
+    <t>Validation Count</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin only.</t>
+  </si>
+  <si>
+    <t>UserAssignment when All unavailable Users in Round Robin only.</t>
+  </si>
+  <si>
+    <t>UserAssignment when All availables Users in Round Robin and All available Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when availables &amp; unavailable Users in Round Robin and available &amp; unavailable Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and all available Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and Unavailable Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and available &amp; unavailable Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and available &amp; unavailable Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available &amp; unavailable Users in Round Robin and  all available Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  all unavailable Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available and unavailable Users in Round Robin and  all unavailable Users in Condition 1.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  all unavailable Users in Condition 1</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  all unavailable Users in Condition 1 and available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  all unavailable Users in Condition 1 and all available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  all available Users in Condition 1 and all unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  all available Users in Condition 1 and available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  all available Users in Condition 1 and all available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  available &amp; unavailable Users in Condition 1 and all unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  available &amp; unavailable Users in Condition 1 and available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all unavailable Users in Round Robin and  available &amp; unavailable Users in Condition 1 and all available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  all unavailable Users in Condition 1 and all unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  all unavailable Users in Condition 1 and available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  all unavailable Users in Condition 1 and all available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  all available Users in Condition 1 and all unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  all available Users in Condition 1 and all available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  all available Users in Condition 1 and all available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  available &amp; unavailable Users in Condition 1 and all available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when all available Users in Round Robin and  available &amp; unavailable Users in Condition 1 and all available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all unavailable Users in Condition 1 and all unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all unavailable Users in Condition 1 and available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all unavailable Users in Condition 1 and available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all available Users in Condition 1 and all unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all available Users in Condition 1 and all available Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all available &amp; unavailable Users in Condition 1 and all unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all available &amp; unavailable Users in Condition 1 and all available &amp; unavailable Users in Condition 2.</t>
+  </si>
+  <si>
+    <t>UserAssignment when available &amp; unavailable Users in Round Robin and  all available &amp; unavailable Users in Condition 1 and all available Users in Condition 2.</t>
   </si>
 </sst>
 </file>
@@ -725,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -754,15 +865,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -777,6 +879,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,7 +1179,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2599,140 +2716,140 @@
         <v>45470</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
+    <row r="21" spans="1:9" s="23" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="23" t="s">
+      <c r="B21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="22">
         <v>45471</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="22">
         <v>45471</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:9" s="23" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="23" t="s">
+      <c r="B22" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="22">
         <v>45471</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="22">
         <v>45471</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A23" s="22" t="s">
+    <row r="23" spans="1:9" s="23" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="23" t="s">
+      <c r="B23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="22">
         <v>45471</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="22">
         <v>45471</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+    <row r="24" spans="1:9" s="23" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="22" t="s">
+      <c r="B24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="22">
         <v>45471</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="22">
         <v>45471</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
+    <row r="25" spans="1:9" s="23" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="27" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="22">
         <v>45471</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="22">
         <v>45471</v>
       </c>
     </row>
@@ -2744,7 +2861,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="18" t="s">
         <v>175</v>
       </c>
       <c r="G26" s="11" t="s">
@@ -2762,7 +2879,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="18" t="s">
         <v>176</v>
       </c>
       <c r="G27" s="11"/>
@@ -2778,7 +2895,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="18" t="s">
         <v>177</v>
       </c>
       <c r="G28" s="3"/>
@@ -2844,7 +2961,7 @@
       <c r="E2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="25">
         <v>45467</v>
       </c>
     </row>
@@ -2864,7 +2981,7 @@
       <c r="E3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -2882,7 +2999,7 @@
       <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
@@ -2900,7 +3017,7 @@
       <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
@@ -2918,7 +3035,7 @@
       <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
@@ -2936,7 +3053,7 @@
       <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3078,48 +3195,500 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="28">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="28">
+        <v>4</v>
+      </c>
+      <c r="D3" s="28">
+        <v>21</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="28">
+        <v>4</v>
+      </c>
+      <c r="D4" s="28">
+        <v>28</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="28">
+        <v>5</v>
+      </c>
+      <c r="D5" s="28">
+        <v>35</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="28">
+        <v>4</v>
+      </c>
+      <c r="D6" s="28">
+        <v>28</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="28">
+        <v>4</v>
+      </c>
+      <c r="D7" s="28">
+        <v>28</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="28">
+        <v>4</v>
+      </c>
+      <c r="D8" s="28">
+        <v>28</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="28">
+        <v>9</v>
+      </c>
+      <c r="D9" s="28">
+        <v>63</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="28">
+        <v>5</v>
+      </c>
+      <c r="D10" s="28">
+        <v>35</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="28">
+        <v>9</v>
+      </c>
+      <c r="D11" s="28">
+        <v>63</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="28">
+        <v>9</v>
+      </c>
+      <c r="D12" s="28">
+        <v>63</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>